<commit_message>
Towers of Hanoi solution
</commit_message>
<xml_diff>
--- a/EPI Problem Tracking.xlsx
+++ b/EPI Problem Tracking.xlsx
@@ -2,31 +2,40 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\EPIJudge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F70E270-8732-4E0E-ADCC-31251FE7D2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFC5276-E25D-4965-81C4-4098C07FC257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Problem</t>
   </si>
@@ -243,6 +252,18 @@
       <t xml:space="preserve">
 4. Use a Queue to do a depth first search in combination with the ranges approach in method 2. Start by adding the root node to a queue, while the queue is not empty, check that the next value falls within its correct range, if it does then add it's children to the queue with their ranges. If any of the items fails to fall within its given range return false. Utilize a customQueueEntry to store the node, and its upper and lower limits for use in the priorityQueue. In the best case this outperforms method 2. TC: O(n), SC: O(n). </t>
     </r>
+  </si>
+  <si>
+    <t>The Towers of Hanoi Problem</t>
+  </si>
+  <si>
+    <t>Difficulty Level</t>
+  </si>
+  <si>
+    <t>Recursion</t>
+  </si>
+  <si>
+    <t>For three pegs do the following to solve the problem: 1. Move all but the last ring from 1 to 3, using 2 as an intermediary. 2. Move the last ring from 1 to 2. 3. Move the remaining rings from 3 to 2 using 1 as an intermediary. Those three steps form the three lines of the recursive portion of the algorithm. In the main function that calls the recursive portion create a list of Stacks (Deque) to mimic the LIFO property of the pegs. Pass the pegs, number of rings, toPeg, from Peg, usingPeg, and result array into the recursive function.  Time complexity: O(2^n)</t>
   </si>
 </sst>
 </file>
@@ -345,15 +366,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3D7E685-48C0-410A-8272-02B5455755F2}" name="Table1" displayName="Table1" ref="A1:F12" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:F12" xr:uid="{A3D7E685-48C0-410A-8272-02B5455755F2}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3D7E685-48C0-410A-8272-02B5455755F2}" name="Table1" displayName="Table1" ref="A1:G13" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:G13" xr:uid="{A3D7E685-48C0-410A-8272-02B5455755F2}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D4BF11D6-B686-4E1D-AD60-C64EE1EBD9D8}" name="Problem"/>
     <tableColumn id="2" xr3:uid="{18BD0209-A429-41AC-93E0-DDA96B17629B}" name="Name"/>
     <tableColumn id="3" xr3:uid="{F45F75B3-19E7-49EF-8ECF-EF1532C83388}" name="Topics"/>
     <tableColumn id="4" xr3:uid="{49297663-BB20-4588-B220-93DC3394241B}" name="Strategies" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{E8FC0EAC-D1DF-4FFB-BBB4-630F2BB6EA0D}" name="Key Insights" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{31070AEE-1431-4BFB-85AE-5892FABDC34B}" name="Time Spent"/>
+    <tableColumn id="6" xr3:uid="{7D771595-5166-4FE3-9FF9-C94982E28346}" name="Difficulty Level"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -622,10 +644,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D18:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +661,7 @@
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,8 +680,11 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5.0999999999999996</v>
       </c>
@@ -675,7 +701,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.6</v>
       </c>
@@ -693,7 +719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6.1</v>
       </c>
@@ -711,7 +737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7.1</v>
       </c>
@@ -729,7 +755,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8.1</v>
       </c>
@@ -747,7 +773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9.1</v>
       </c>
@@ -765,7 +791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10.1</v>
       </c>
@@ -783,7 +809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11.1</v>
       </c>
@@ -801,7 +827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12.1</v>
       </c>
@@ -819,7 +845,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>13.1</v>
       </c>
@@ -836,7 +862,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="285" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="285" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>14.1</v>
       </c>
@@ -851,6 +877,24 @@
       </c>
       <c r="E12" s="2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>15.1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="G13">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
My solutions to additional EPI problems
</commit_message>
<xml_diff>
--- a/EPI Problem Tracking.xlsx
+++ b/EPI Problem Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\EPIJudge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFC5276-E25D-4965-81C4-4098C07FC257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9E49A5-C910-4806-AC8B-7EAD7E85E500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Problem</t>
   </si>
@@ -264,6 +264,11 @@
   </si>
   <si>
     <t>For three pegs do the following to solve the problem: 1. Move all but the last ring from 1 to 3, using 2 as an intermediary. 2. Move the last ring from 1 to 2. 3. Move the remaining rings from 3 to 2 using 1 as an intermediary. Those three steps form the three lines of the recursive portion of the algorithm. In the main function that calls the recursive portion create a list of Stacks (Deque) to mimic the LIFO property of the pegs. Pass the pegs, number of rings, toPeg, from Peg, usingPeg, and result array into the recursive function.  Time complexity: O(2^n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To generate the three stacks needed for the three pegs, use this cool piece of code:
+List&lt;Deque&lt;Integer&gt;&gt; pegs = IntStream.range(0, NUM_PEGS).mapToObj(i-&gt; new ArrayDeque&lt;Integer&gt;()).collect(Collectors.toList());
+</t>
   </si>
 </sst>
 </file>
@@ -648,7 +653,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D18:D19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +897,9 @@
       <c r="D13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="G13">
         <v>3</v>
       </c>

</xml_diff>